<commit_message>
added images and report
</commit_message>
<xml_diff>
--- a/data/thrust_test.xlsx
+++ b/data/thrust_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kushal\propeller_balancer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BTech IITB\BTP\propeller_balancer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B864992-7181-4A89-95E1-30DD5159BE70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C83A33C-ED8B-404F-97E7-D6EBAE6B4F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{B767E155-44C8-4508-B44C-6776177F224E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{B767E155-44C8-4508-B44C-6776177F224E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,6 +341,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>motor speed</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -403,6 +463,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Thrust (g)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1393,32 +1508,32 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1426,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1434,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1442,7 +1557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>15</v>
       </c>
@@ -1450,7 +1565,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>20</v>
       </c>
@@ -1458,7 +1573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>25</v>
       </c>
@@ -1466,7 +1581,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>30</v>
       </c>
@@ -1474,7 +1589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>35</v>
       </c>
@@ -1482,7 +1597,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>40</v>
       </c>
@@ -1490,12 +1605,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1506,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1517,7 +1632,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1528,7 +1643,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>15</v>
       </c>
@@ -1539,7 +1654,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1550,7 +1665,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>25</v>
       </c>
@@ -1561,7 +1676,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>30</v>
       </c>
@@ -1572,7 +1687,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>35</v>
       </c>
@@ -1583,7 +1698,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>40</v>
       </c>
@@ -1594,12 +1709,12 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1610,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1621,7 +1736,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1632,7 +1747,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -1643,7 +1758,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>20</v>
       </c>
@@ -1654,7 +1769,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>25</v>
       </c>
@@ -1665,7 +1780,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>30</v>
       </c>
@@ -1676,7 +1791,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1687,7 +1802,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>40</v>
       </c>
@@ -1698,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>45</v>
       </c>

</xml_diff>